<commit_message>
finished agile backlog v1.2
</commit_message>
<xml_diff>
--- a/Documents/Agile Project Management -Backlog.xlsx
+++ b/Documents/Agile Project Management -Backlog.xlsx
@@ -1012,24 +1012,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFADCB3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1051,19 +1061,19 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFF6600"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1085,23 +1095,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFCC00"/>
@@ -1119,104 +1112,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1254,16 +1152,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1352,26 +1240,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1508,151 +1376,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1724,61 +1447,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>212</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>203</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>198</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>194</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>185</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>180</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>176</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>171</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>167</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>163</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>158</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>154</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>150</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>146</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>141</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>137</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>133</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1790,49 +1513,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>217</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>209</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>178</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>168</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>140</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>103</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>76</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>59</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>34</c:v>
@@ -1858,11 +1581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1275198256"/>
-        <c:axId val="-1275197168"/>
+        <c:axId val="-1890594768"/>
+        <c:axId val="-1890600208"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1275198256"/>
+        <c:axId val="-1890594768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +1614,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-1275197168"/>
+        <c:crossAx val="-1890600208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1899,7 +1622,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1275197168"/>
+        <c:axId val="-1890600208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1944,7 +1667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275198256"/>
+        <c:crossAx val="-1890594768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2286,10 +2009,10 @@
   <dimension ref="A1:AC139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V57" sqref="V57"/>
+      <selection pane="bottomRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3805,7 +3528,7 @@
       <c r="G29" s="43">
         <v>7</v>
       </c>
-      <c r="H29" s="60">
+      <c r="H29" s="58">
         <f t="shared" ref="H29" si="2">IF((G29&lt;SUM(J29:AA29)),SUM(J29:AA29),G29)</f>
         <v>7</v>
       </c>
@@ -3856,9 +3579,15 @@
       <c r="F30" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="16"/>
+      <c r="G30" s="43">
+        <v>6</v>
+      </c>
+      <c r="H30" s="58">
+        <v>6</v>
+      </c>
+      <c r="I30" s="16">
+        <v>0</v>
+      </c>
       <c r="J30" s="47"/>
       <c r="K30" s="48"/>
       <c r="L30" s="48"/>
@@ -3871,9 +3600,13 @@
       <c r="S30" s="48"/>
       <c r="T30" s="48"/>
       <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
+      <c r="V30" s="48">
+        <v>4</v>
+      </c>
       <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
+      <c r="X30" s="48">
+        <v>2</v>
+      </c>
       <c r="Y30" s="48"/>
       <c r="Z30" s="48"/>
       <c r="AA30" s="49"/>
@@ -3896,9 +3629,15 @@
       <c r="F31" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="16"/>
+      <c r="G31" s="43">
+        <v>5</v>
+      </c>
+      <c r="H31" s="58">
+        <v>5</v>
+      </c>
+      <c r="I31" s="16">
+        <v>0</v>
+      </c>
       <c r="J31" s="47"/>
       <c r="K31" s="48"/>
       <c r="L31" s="48"/>
@@ -3910,9 +3649,13 @@
       <c r="R31" s="48"/>
       <c r="S31" s="48"/>
       <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
+      <c r="U31" s="48">
+        <v>3</v>
+      </c>
       <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
+      <c r="W31" s="48">
+        <v>2</v>
+      </c>
       <c r="X31" s="48"/>
       <c r="Y31" s="48"/>
       <c r="Z31" s="48"/>
@@ -3936,9 +3679,15 @@
       <c r="F32" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="16"/>
+      <c r="G32" s="43">
+        <v>8</v>
+      </c>
+      <c r="H32" s="58">
+        <v>8</v>
+      </c>
+      <c r="I32" s="16">
+        <v>0</v>
+      </c>
       <c r="J32" s="47"/>
       <c r="K32" s="48"/>
       <c r="L32" s="48"/>
@@ -3951,9 +3700,13 @@
       <c r="S32" s="48"/>
       <c r="T32" s="48"/>
       <c r="U32" s="48"/>
-      <c r="V32" s="48"/>
+      <c r="V32" s="48">
+        <v>4</v>
+      </c>
       <c r="W32" s="48"/>
-      <c r="X32" s="48"/>
+      <c r="X32" s="48">
+        <v>4</v>
+      </c>
       <c r="Y32" s="48"/>
       <c r="Z32" s="48"/>
       <c r="AA32" s="49"/>
@@ -5818,11 +5571,11 @@
       <c r="F73" s="25"/>
       <c r="G73" s="26">
         <f>SUM(G3:G72)</f>
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="H73" s="27">
         <f>SUM(H3:H72)</f>
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="I73" s="27">
         <f>SUM(I3:I72)</f>
@@ -5874,19 +5627,19 @@
       </c>
       <c r="U73" s="28">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="V73" s="28">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="W73" s="28">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="X73" s="28">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="Y73" s="28">
         <f t="shared" si="8"/>
@@ -5912,7 +5665,7 @@
       <c r="F74" s="31"/>
       <c r="G74" s="32">
         <f>G73-SUM(J74:AA74)</f>
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="H74" s="33"/>
       <c r="I74" s="34"/>
@@ -5982,79 +5735,79 @@
       </c>
       <c r="I75" s="37">
         <f>G73</f>
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="J75" s="39">
         <f t="shared" ref="J75:AA75" si="9">I75-J74</f>
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="K75" s="39">
         <f t="shared" si="9"/>
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="L75" s="39">
         <f t="shared" si="9"/>
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="M75" s="39">
         <f t="shared" si="9"/>
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="N75" s="39">
         <f t="shared" si="9"/>
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="O75" s="39">
         <f t="shared" si="9"/>
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="P75" s="39">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="Q75" s="39">
         <f t="shared" si="9"/>
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="R75" s="39">
         <f t="shared" si="9"/>
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="S75" s="39">
         <f t="shared" si="9"/>
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="T75" s="39">
         <f t="shared" si="9"/>
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="U75" s="39">
         <f t="shared" si="9"/>
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="V75" s="39">
         <f t="shared" si="9"/>
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="W75" s="39">
         <f t="shared" si="9"/>
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="X75" s="39">
         <f t="shared" si="9"/>
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="Y75" s="39">
         <f t="shared" si="9"/>
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="Z75" s="39">
         <f>Y75-Z74</f>
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="AA75" s="39">
         <f t="shared" si="9"/>
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -6068,63 +5821,63 @@
       </c>
       <c r="I76" s="37">
         <f>H73</f>
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="J76" s="37">
         <f>$H$73-SUM(J$3:J$72)</f>
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="K76" s="37">
         <f t="shared" ref="K76:AA76" si="10">J76-SUM(K3:K72)</f>
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="L76" s="37">
         <f t="shared" si="10"/>
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="M76" s="37">
         <f t="shared" si="10"/>
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="N76" s="37">
         <f t="shared" si="10"/>
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="O76" s="37">
         <f t="shared" si="10"/>
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="P76" s="37">
         <f t="shared" si="10"/>
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="Q76" s="37">
         <f t="shared" si="10"/>
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="R76" s="37">
         <f t="shared" si="10"/>
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="S76" s="37">
         <f t="shared" si="10"/>
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="T76" s="37">
         <f t="shared" si="10"/>
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="U76" s="37">
         <f t="shared" si="10"/>
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="V76" s="37">
         <f t="shared" si="10"/>
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="W76" s="37">
         <f t="shared" si="10"/>
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="X76" s="37">
         <f t="shared" si="10"/>
@@ -6144,11 +5897,11 @@
       </c>
     </row>
     <row r="77" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E77" s="58"/>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="58"/>
-      <c r="I77" s="58"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="59"/>
       <c r="K77" s="35"/>
       <c r="L77" s="35"/>
       <c r="M77" s="35"/>
@@ -6168,11 +5921,11 @@
       <c r="AA77" s="35"/>
     </row>
     <row r="78" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="E78" s="59"/>
-      <c r="F78" s="59"/>
-      <c r="G78" s="59"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="59"/>
+      <c r="E78" s="60"/>
+      <c r="F78" s="60"/>
+      <c r="G78" s="60"/>
+      <c r="H78" s="60"/>
+      <c r="I78" s="60"/>
       <c r="K78" s="35"/>
       <c r="L78" s="35"/>
       <c r="M78" s="35"/>
@@ -6441,207 +6194,198 @@
     <mergeCell ref="E78:I78"/>
   </mergeCells>
   <conditionalFormatting sqref="E75:E76 H75:AA76">
-    <cfRule type="cellIs" dxfId="56" priority="39" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="39" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74">
-    <cfRule type="cellIs" dxfId="55" priority="40" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="40" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I15 I59:I72">
-    <cfRule type="cellIs" dxfId="54" priority="41" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="41" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="41" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="41" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="41" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:F74 I74">
-    <cfRule type="cellIs" dxfId="51" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="42" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="42" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="42" stopIfTrue="1" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:AA15 J59:AA72">
-    <cfRule type="cellIs" dxfId="49" priority="43" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="43" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74">
-    <cfRule type="cellIs" dxfId="48" priority="44" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="44" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="44" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="44" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F75:G76">
-    <cfRule type="cellIs" dxfId="46" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="37" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I28 I33:I53 I58">
-    <cfRule type="cellIs" dxfId="45" priority="33" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="33" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:AA28 J33:AA53 J58:AA58">
-    <cfRule type="cellIs" dxfId="44" priority="34" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="34" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I28">
-    <cfRule type="cellIs" dxfId="43" priority="32" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="32" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:AA28">
-    <cfRule type="cellIs" dxfId="42" priority="31" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="31" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48:I53">
-    <cfRule type="cellIs" dxfId="41" priority="30" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="30" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:AA53">
-    <cfRule type="cellIs" dxfId="40" priority="29" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="29" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 I32">
-    <cfRule type="cellIs" dxfId="39" priority="-1" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="-1" stopIfTrue="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="26" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="26" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:AA29 J32:AA32">
-    <cfRule type="cellIs" dxfId="36" priority="25" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="25" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="35" priority="23" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:AA54">
-    <cfRule type="cellIs" dxfId="34" priority="24" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="24" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="33" priority="22" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="22" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:AA54">
-    <cfRule type="cellIs" dxfId="32" priority="21" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="21" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="cellIs" dxfId="31" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="19" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:AA31">
-    <cfRule type="cellIs" dxfId="28" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="27" priority="-1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="15" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:AA30">
-    <cfRule type="cellIs" dxfId="24" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="cellIs" dxfId="23" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:AA55">
-    <cfRule type="cellIs" dxfId="21" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="cellIs" dxfId="19" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:AA55">
-    <cfRule type="cellIs" dxfId="17" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56">
-    <cfRule type="cellIs" dxfId="15" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:AA56">
-    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56">
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:AA56">
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:AA57">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:AA57">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>